<commit_message>
Finished car filtering Workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\UiPath\Cars_on_Mobile\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Cars_on_Mobile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE0B7C4-3FFB-4F5D-84B8-3CAE76624EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440D8F2B-4D60-49B1-8CFF-1D5DB85659FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -64,6 +64,30 @@
   </si>
   <si>
     <t>Estate Car;Saloon;Sports Car / Coupe</t>
+  </si>
+  <si>
+    <t>seatsNumber</t>
+  </si>
+  <si>
+    <t>fuelType</t>
+  </si>
+  <si>
+    <t>Diesel;Petrol</t>
+  </si>
+  <si>
+    <t>powerNumber</t>
+  </si>
+  <si>
+    <t>cubicCapacity</t>
+  </si>
+  <si>
+    <t>transmissionType</t>
+  </si>
+  <si>
+    <t>Manual Gearbox</t>
+  </si>
+  <si>
+    <t>emissionSticker</t>
   </si>
 </sst>
 </file>
@@ -411,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,6 +498,54 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{B3205F37-17A9-4DAD-A748-77A163AEE172}"/>

</xml_diff>

<commit_message>
Applied all filter on workbook. Put everything together. Minor bug fixes and changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Cars_on_Mobile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440D8F2B-4D60-49B1-8CFF-1D5DB85659FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D959E9F-00AD-4DA3-A5B0-3FE558DC90CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Link for 'mobile.de' website</t>
   </si>
   <si>
-    <t>BrowserProcess</t>
-  </si>
-  <si>
     <t>msedge</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>seatsNumber</t>
   </si>
   <si>
-    <t>fuelType</t>
-  </si>
-  <si>
     <t>Diesel;Petrol</t>
   </si>
   <si>
@@ -84,10 +78,34 @@
     <t>transmissionType</t>
   </si>
   <si>
-    <t>Manual Gearbox</t>
-  </si>
-  <si>
     <t>emissionSticker</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>emailReceiver</t>
+  </si>
+  <si>
+    <t>emailSubject</t>
+  </si>
+  <si>
+    <t>Car List</t>
+  </si>
+  <si>
+    <t>browserProcess</t>
+  </si>
+  <si>
+    <t>fuelTypes</t>
+  </si>
+  <si>
+    <t>Manual gearbox</t>
+  </si>
+  <si>
+    <t>Data\Output\OutputReport</t>
+  </si>
+  <si>
+    <t>patricia.ciortin@fwfcompany.com;calin.gandila@fwfcompany.com;diana.sacacian@fwfcompany.com</t>
   </si>
 </sst>
 </file>
@@ -146,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -154,6 +172,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,13 +481,13 @@
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -476,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -484,23 +503,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -508,15 +527,15 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>131</v>
@@ -524,7 +543,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>3000</v>
@@ -532,18 +551,42 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>